<commit_message>
added dataprovider with excel functions
</commit_message>
<xml_diff>
--- a/src/test/java/com/framework/tests/testData.xlsx
+++ b/src/test/java/com/framework/tests/testData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -37,10 +37,73 @@
     <t xml:space="preserve">Weight</t>
   </si>
   <si>
-    <t xml:space="preserve">Skintone</t>
-  </si>
-  <si>
     <t xml:space="preserve">Gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rajesh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'test45@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">‘45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">170</t>
+  </si>
+  <si>
+    <t xml:space="preserve">65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sabari</t>
+  </si>
+  <si>
+    <t xml:space="preserve">‘46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">171</t>
+  </si>
+  <si>
+    <t xml:space="preserve">66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">‘47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172</t>
+  </si>
+  <si>
+    <t xml:space="preserve">67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">navin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">‘48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">173</t>
+  </si>
+  <si>
+    <t xml:space="preserve">68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aro </t>
+  </si>
+  <si>
+    <t xml:space="preserve">‘49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">174</t>
+  </si>
+  <si>
+    <t xml:space="preserve">69</t>
   </si>
 </sst>
 </file>
@@ -50,7 +113,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -71,6 +134,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -115,8 +185,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -137,38 +215,142 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="test45@gmail.com"/>
+    <hyperlink ref="B3" r:id="rId2" display="test45@gmail.com"/>
+    <hyperlink ref="B4" r:id="rId3" display="test45@gmail.com"/>
+    <hyperlink ref="B5" r:id="rId4" display="test45@gmail.com"/>
+    <hyperlink ref="B6" r:id="rId5" display="test45@gmail.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>